<commit_message>
Added more benchmark resutls
</commit_message>
<xml_diff>
--- a/data/all_results.xlsx
+++ b/data/all_results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindemann/Documents/rviz_report/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas_000\Documents\rviz_report\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NVIDIA Performance" sheetId="2" r:id="rId1"/>
     <sheet name="GpuTest VNC Performance (FPS)" sheetId="3" r:id="rId2"/>
     <sheet name="all_results.csv" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -121,6 +121,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -128,7 +131,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -165,7 +168,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -305,94 +308,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>71.0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.0</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>257.0</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69.0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>97.0</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +410,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-2141912592"/>
-        <c:axId val="-2141908912"/>
+        <c:axId val="1900554608"/>
+        <c:axId val="1900555152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141912592"/>
+        <c:axId val="1900554608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,10 +454,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141908912"/>
+        <c:crossAx val="1900555152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -462,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141908912"/>
+        <c:axId val="1900555152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,10 +513,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141912592"/>
+        <c:crossAx val="1900554608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -551,7 +554,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sv-SE"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -560,7 +563,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sv-SE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -578,19 +581,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -598,13 +595,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>GpuTest</a:t>
+              <a:t>GpuTest VNC Performance (FPS)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> VNC Performance (FPS)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -622,25 +614,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -666,42 +652,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -721,8 +678,9 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -730,10 +688,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sv-SE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -747,13 +705,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="95000"/>
-                          <a:alpha val="54000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -794,22 +753,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>71.0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,42 +789,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -885,8 +815,9 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -894,10 +825,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sv-SE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -911,13 +842,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="95000"/>
-                          <a:alpha val="54000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -958,22 +890,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>67.0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,42 +926,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1049,8 +952,9 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1058,10 +962,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sv-SE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1075,13 +979,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="95000"/>
-                          <a:alpha val="54000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1122,22 +1027,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1158,42 +1063,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1213,8 +1089,9 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1222,10 +1099,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sv-SE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1239,13 +1116,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="95000"/>
-                          <a:alpha val="54000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1286,22 +1164,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>85.0</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,42 +1200,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -1377,8 +1226,9 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1386,10 +1236,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sv-SE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1403,13 +1253,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="95000"/>
-                          <a:alpha val="54000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1450,29 +1301,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>257.0</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.0</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1480,12 +1331,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:axId val="-2141722192"/>
-        <c:axId val="-2141718896"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1640255088"/>
+        <c:axId val="1640243120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141722192"/>
+        <c:axId val="1640255088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,11 +1349,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1515,8 +1367,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1524,10 +1377,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141718896"/>
+        <c:crossAx val="1640243120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1535,7 +1388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141718896"/>
+        <c:axId val="1640243120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,9 +1398,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1573,8 +1426,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1582,10 +1436,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141722192"/>
+        <c:crossAx val="1640255088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1615,8 +1469,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1624,7 +1479,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1633,28 +1488,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1665,7 +1509,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sv-SE"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2257,33 +2101,35 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2291,34 +2137,26 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2327,8 +2165,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2347,6 +2186,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2355,35 +2202,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2395,31 +2242,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2435,18 +2281,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2456,20 +2305,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2480,17 +2329,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2499,13 +2348,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2517,22 +2367,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2544,103 +2400,96 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2648,14 +2497,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2667,19 +2516,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2688,13 +2530,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2703,8 +2546,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2714,7 +2558,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2722,9 +2566,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2735,8 +2579,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2746,8 +2591,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2767,10 +2618,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2805,7 +2657,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9301151" cy="6066763"/>
+    <xdr:ext cx="8662883" cy="6292062"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3097,20 +2949,20 @@
       <selection activeCell="J3" sqref="J3:O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="28.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="2" max="5" width="28.625" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
+    <col min="13" max="13" width="14.125" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1024</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3159,7 +3011,7 @@
         <v>TessMark</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3211,7 +3063,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3263,7 +3115,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3167,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3367,7 +3219,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3419,7 +3271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3471,7 +3323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3499,7 +3351,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3527,7 +3379,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3555,7 +3407,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3583,7 +3435,7 @@
         <v>3953</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -3611,7 +3463,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3639,7 +3491,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3667,7 +3519,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3695,7 +3547,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3723,7 +3575,7 @@
         <v>4194</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3751,7 +3603,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3779,7 +3631,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3807,7 +3659,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3835,7 +3687,7 @@
         <v>2535</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3863,7 +3715,7 @@
         <v>5851</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3891,7 +3743,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -3919,7 +3771,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3799,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -3975,7 +3827,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -4003,7 +3855,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4031,7 +3883,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -4059,7 +3911,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -4087,7 +3939,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -4115,7 +3967,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>

</xml_diff>